<commit_message>
updated glossary and EA file according to some GitHub issues
</commit_message>
<xml_diff>
--- a/v2.0.1/02-Glossary/ePO-Glossary.xlsx
+++ b/v2.0.1/02-Glossary/ePO-Glossary.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1344" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1317" uniqueCount="538">
   <si>
     <t>ClassName</t>
   </si>
@@ -379,8 +379,7 @@
 (WG approval 22/06/2018)</t>
   </si>
   <si>
-    <t>The provision which confers competence to adopt the act in question.
-(Pending to review by the WG)</t>
+    <t>The provision which confers competence to adopt the act in question.</t>
   </si>
   <si>
     <t>The value  provided for a criterion property.
@@ -391,8 +390,7 @@
 WG 12/09/2018</t>
   </si>
   <si>
-    <t>Members of an evaluation committee (e.g..: jury members) that take into account the requirements, specifications and conditions of the tenders in order to evaluate them. 
-(Pending to review by the WG)</t>
+    <t>Members of an evaluation committee (e.g..: jury members) that take into account the requirements, specifications and conditions of the tenders in order to evaluate them.</t>
   </si>
   <si>
     <t>Describes a rule or a condition to be taken into account for the award decision.
@@ -409,7 +407,7 @@
   </si>
   <si>
     <t>Organisation that manages the budget allocated for the procedure and pays for the items being procured.
-WG  14/11/2018</t>
+WG Approval  14/11/2018</t>
   </si>
   <si>
     <t>Website address where the buyer publishes information on its procurement procedures and general information.
@@ -420,8 +418,7 @@
 (WG approval 14/05/2017)</t>
   </si>
   <si>
-    <t>A call to potential providers of goods and/or services to register interest in supplying them. It is a document that describes a set of requirements or specifications and that service providers have to demonstrate their ability to meet those requirements. 
-(Pending to review by the WG)</t>
+    <t>A call to potential providers of goods and/or services to register interest in supplying them. It is a document that describes a set of requirements or specifications and that service providers have to demonstrate their ability to meet those requirements.</t>
   </si>
   <si>
     <t>The tenderers that have been selected in a two stage procedure.
@@ -437,12 +434,7 @@
 (WG approval 01/06/2018)</t>
   </si>
   <si>
-    <t>An announcement of the award or non-award of a contract by a procuring entity.
-(WG approval 27/03/2019 9:41:42)</t>
-  </si>
-  <si>
-    <t>An announcement of the modification of a contract/concession during during its term by a procuring entity.
-(Pending to review by the WG)</t>
+    <t>An announcement of the modification of a contract/concession during during its term by a procuring entity.</t>
   </si>
   <si>
     <t>An announcement of the launch of a procurement procedure by a procuring entity.
@@ -450,7 +442,10 @@
   </si>
   <si>
     <t>Conditions and stipulations defining particularities of the post award phase.
-(WG decision 23/11/2018)</t>
+(WG approval 23/11/2018)</t>
+  </si>
+  <si>
+    <t>Describes the object of the procurement and the properties of the procedure.</t>
   </si>
   <si>
     <t>An electronic system that is set up by a procuring entity which lists the economic operators that satisfy the selection and exclusion criteria.   This technique then allows the purchase via consultation of the listed tenderers using award criteria.
@@ -484,16 +479,13 @@
 WG Approval 2019-02-05</t>
   </si>
   <si>
-    <t>European Single Procurement Document Request. Specification by the Procuring Entity of the exclusion and selection criteria for a Procurement Procedure. 
-(Pending to review by the WG)</t>
-  </si>
-  <si>
-    <t>European Single Procurement Document Response. The declaration of the Economic Operator that it meets all the exclusion and selection criteria specified in the ESPD Request.
-(Pending to review by the WG)</t>
-  </si>
-  <si>
-    <t>The Evaluation Board publishes the result of tenders after completion of its evaluation.
-(Pending to review by the WG)</t>
+    <t>European Single Procurement Document Request. Specification by the Procuring Entity of the exclusion and selection criteria for a Procurement Procedure.</t>
+  </si>
+  <si>
+    <t>European Single Procurement Document Response. The declaration of the Economic Operator that it meets all the exclusion and selection criteria specified in the ESPD Request.</t>
+  </si>
+  <si>
+    <t>The Evaluation Board publishes the result of tenders after completion of its evaluation.</t>
   </si>
   <si>
     <t>An automated solution that assesses structured information in tenders and proposes results.
@@ -539,22 +531,17 @@
 Additional Information:
 The non-published information may become available at a later date and may differ from one element to another within a given document.
 Examples of fields that may not be immediately published are Winner, Tender and Procedure Lot Result, etc., e.g. for security reasons.
-WG Approve 16/05/2019</t>
-  </si>
-  <si>
-    <t>Notification or a formal declaration of someone's intention to end an agreement, typically one concerning employment or tenancy, at a specified time.
-(Pending to review by the WG)</t>
+WG Approval 16/05/2019</t>
+  </si>
+  <si>
+    <t>Notification or a formal declaration of someone's intention to end an agreement, typically one concerning employment or tenancy, at a specified time.</t>
   </si>
   <si>
     <t>The language(s) in which these procurement documents are officially available. These linguistic versions are equally legally valid.
-WG Approval 07/03/2019 15:31:58</t>
-  </si>
-  <si>
-    <t>(Pending to review by the WG)</t>
-  </si>
-  <si>
-    <t>Notice which sets out the contracting authority's purchasing intentions. It is used by contracting authorities to provide suppliers with information about a procurement process. 
-(Pending to review by the WG)</t>
+WG Approval 07/03/2019</t>
+  </si>
+  <si>
+    <t>Notice which sets out the contracting authority's purchasing intentions. It is used by contracting authorities to provide suppliers with information about a procurement process.</t>
   </si>
   <si>
     <t>A series of legally defined administrative steps conducted  to conclude one or more contracts.
@@ -569,8 +556,7 @@
 (WG approval 07/11/2018)</t>
   </si>
   <si>
-    <t>Statistical data on the procedure and the lot. Also used to emphasize the suitability of the procurement for the SMEs or other purposes.
-Pending to review by the WG</t>
+    <t>Statistical data on the procedure and the lot. Also used to emphasize the suitability of the procurement for the SMEs or other purposes.</t>
   </si>
   <si>
     <t>Monetary amount related to a procurement.
@@ -599,23 +585,21 @@
   <si>
     <t>Condition that aims to reduce the environmental impacts of the procurement, fulfil social objectives and/or buy an innovative work, supply or service.
 Additional Information: The conditions must be achieved via either  technical specifications, selection criteria, award criteria and contract terms.
-WG Approval 02/04/2019 15:39:57</t>
+WG Approval 02/04/2019</t>
   </si>
   <si>
     <t>A contract between a contractor of an original contract and another economic operator to fulfil the original contract.
 WG Approval 07/05/2019</t>
   </si>
   <si>
-    <t>A concept to describe the main information regarding the share of parts of the contract to third parties.
-(Pending to review by the WG)</t>
+    <t>A concept to describe the main information regarding the share of parts of the contract to third parties.</t>
   </si>
   <si>
     <t>Use of electronic submission.
-WG Approval 07/03/2019 16:45:58</t>
-  </si>
-  <si>
-    <t>Method by which a procurement contract is established.
-(Pending to review by the WG)</t>
+WG Approval 07/03/2019</t>
+  </si>
+  <si>
+    <t>Method by which a procurement contract is established.</t>
   </si>
   <si>
     <t>Information submitted by the economic operator to specify its offer regarding one or more lots or the whole procedure, in response to the call for tender.
@@ -627,7 +611,11 @@
   </si>
   <si>
     <t>The procurement documents (or their parts) are also available in the following languages. These versions are not an official translation, they are provided only for information.
-WG Approval 07/03/2019 15:33:37</t>
+WG Approval 07/03/2019</t>
+  </si>
+  <si>
+    <t>The tenderer to whom the contract is awarded.
+(WG approval 20/11/2018)</t>
   </si>
   <si>
     <t>A collection of people organized together into a community or other social, commercial or political structure. The group has some common purpose or reason for existence which goes beyond the set of people belonging to it and can act as an Agent. Organizations are often decomposable into hierarchical structures.
@@ -1382,12 +1370,11 @@
 Local</t>
   </si>
   <si>
-    <t>The category of the criterion whether it be concerned with the quality of the offer or the financial offer.
-(Pending to review by the WG)</t>
+    <t>The category of the criterion whether it be concerned with the quality of the offer or the financial offer.</t>
   </si>
   <si>
     <t>An indication whether any tenderer has been chosen for a contract or framework agreement.
-WG Approval 19/03/2019 15:57:43</t>
+WG Approval 19/03/2019</t>
   </si>
   <si>
     <t>The justification for using a procedure which allows directly awarding contracts.
@@ -1421,34 +1408,30 @@
     <t>The maximum number of contract extensions foreseen for this contract.</t>
   </si>
   <si>
-    <t>Indicates whether subsequent service contracts will be awarded to the winner or one of the winners of a design contest by a negotiated procedure without publication.
-(Pending to review by the WG)</t>
+    <t>Indicates whether subsequent service contracts will be awarded to the winner or one of the winners of a design contest by a negotiated procedure without publication.</t>
   </si>
   <si>
     <t>The particular conditions and additional information related to the execution of the contract.
 Additional Information: e.g. specific information about the place of performance, intermediary deliverables, compensation for damages, intellectual property rights.
-(WG approved 15-01-2019)</t>
-  </si>
-  <si>
-    <t>Electronic means are used for requesting and purchasing in the post-award process.
-(Pending to review by the WG)</t>
-  </si>
-  <si>
-    <t>Electronic means are used for paying the winner of the contract in the post-award process.
-(Pending to review by the WG)</t>
+(WG approval 15-01-2019)</t>
+  </si>
+  <si>
+    <t>Electronic means are used for requesting and purchasing in the post-award process.</t>
+  </si>
+  <si>
+    <t>Electronic means are used for paying the winner of the contract in the post-award process.</t>
   </si>
   <si>
     <t>Any other information about the renewal(s).
-WG approval 16/04/2019 15:01:09</t>
+WG approval 16/04/2019</t>
   </si>
   <si>
     <t>A specific legal entity must be taken up by a tenderer composed of a group of economic operators once it has been awarded a contract.
 Additional information: this may be applied in the case of groups (e.g. a consortium) where the requirement is that they have to formalise the relationship of the group members as a legal entity itself once the contract is awarded.
-WG Approval 2019-01-29, 2019-01-30</t>
-  </si>
-  <si>
-    <t>A constraint concerning the legal form that must be adopted by a tenderer composed of a group of economic operators once it has been awarded a contract.
-CONCEPT UNDER DISCUSSION WITH eForms and WG</t>
+WG Approval 2019-01-29</t>
+  </si>
+  <si>
+    <t>A constraint concerning the legal form that must be adopted by a tenderer composed of a group of economic operators once it has been awarded a contract.</t>
   </si>
   <si>
     <t>Information about financial clauses that will govern some economic aspects of the execution of the contract.
@@ -1470,8 +1453,7 @@
   </si>
   <si>
     <t>Access to procurement document is restricted.
-The property Document.Restricted Access of type code is kept for now as it is interesting that a document confidentiality policy is self contained in the document but we need to address the consistency with the Access Restriction indicator property.
-To be reviewed (07/03/2019 15:40:05)</t>
+The property Document.Restricted Access of type code is kept for now as it is interesting that a document confidentiality policy is self contained in the document but we need to address the consistency with the Access Restriction indicator property.</t>
   </si>
   <si>
     <t>Closure of the DPS. 
@@ -1501,7 +1483,6 @@
   </si>
   <si>
     <t>The number of solutions or tenders will be reduced in iterative evaluations for multiple staged procedures.
-(Pending to review by the WG)
 Additional information:
 This refers to multiple-stage procedures (included two-stage procedures, at least). Open Procedures can be seen as one-stage procedures. In multiple-stage procedure the first stage (or round) is used for the selection of the candidates, whilst the rest of stages is about submitting tenders and warning (or not) about the right of the CA to award without further negotiations. See Article 29(4) of Directive 2014/24/EU.</t>
   </si>
@@ -1521,9 +1502,6 @@
 Overall award criteria Weight 20% Price, 60% Quality, 20% Cost</t>
   </si>
   <si>
-    <t>WG Approval 23-01-2019</t>
-  </si>
-  <si>
     <t>A country is one of the political units which the world is divided into, covering a particular area of land.
 (WG approval 8/06/2018)</t>
   </si>
@@ -1533,8 +1511,7 @@
 WG Approval 2019-05-06</t>
   </si>
   <si>
-    <t>In the case of a framework agreement, the reasons for any duration exceeding four years.
-(Pending to review by the WG)</t>
+    <t>In the case of a framework agreement, the reasons for any duration exceeding four years.</t>
   </si>
   <si>
     <t>Maximum number of tenderers who may be awarded a contract within the framework agreement.
@@ -1542,23 +1519,25 @@
 WG Approval 2019-02-05</t>
   </si>
   <si>
-    <t>The participation is reserved to organisations pursuing a public service mission and fulfilling other relevant conditions in the legislation.
-WG TBD</t>
-  </si>
-  <si>
-    <t>The date when a record is made publically available.
+    <t>The participation is reserved to organisations pursuing a public service mission and fulfilling other relevant conditions in the legislation.</t>
+  </si>
+  <si>
+    <t>The date when a record is made publicly available.
 (WG approval 01/06/2018)</t>
   </si>
   <si>
     <t>Date and time for the opening of tenders.
-WG Approval 12/03/2019 16:11:39</t>
-  </si>
-  <si>
-    <t>Further information about the opening of tenders. (For example, who may participate in the opening and whether any authorisation is needed.)
-WG Approval 12/03/2019 16:10:50</t>
-  </si>
-  <si>
-    <t>Specifies whether the GPA applies.
+WG Approval 12/03/2019</t>
+  </si>
+  <si>
+    <t>Further information about the opening of tenders. (For example, who may participate in the opening and whether any authorization is needed.)
+WG Approval 12/03/2019</t>
+  </si>
+  <si>
+    <t>Explanation about why the choice of an accelerated procedure is lawful.</t>
+  </si>
+  <si>
+    <t>Specifies whether the Agreement on Government Procurement (GPA) applies.
 Additional information: the GPA aims to establish a multilateral framework of balanced rights and obligations relating to public contracts with a view to achieving the liberalization and expansion of world trade.
 Reason: the ISO/IEC 11179 Recommends not to over-define the terms but instead to separate extra information when the general concept (in this case GPA) is not defined in the glossary.</t>
   </si>
@@ -1570,8 +1549,8 @@
 (WG approval 01/06/2018)</t>
   </si>
   <si>
-    <t>The total number of lots for which one tenderer can submit tenders..
-(WG decision 12/12/2018)</t>
+    <t>The total number of lots for which one tenderer can submit tenders.
+(WG approval 12/12/2018)</t>
   </si>
   <si>
     <t>No further contracts will be awarded in this competition.
@@ -1579,69 +1558,59 @@
 Additional Information: PIN for Competition and DPS, for example, are cases where the termination needs to be signaled.</t>
   </si>
   <si>
-    <t>Estimated time of transmission of invitation to submit tenders.
-(Pending to review by the WG)</t>
-  </si>
-  <si>
-    <t>Time limit for receipt of expressions of interest.
-(Pending to review by the WG)</t>
+    <t>Estimated time of transmission of invitation to submit tenders.</t>
+  </si>
+  <si>
+    <t>Time limit for receipt of expressions of interest.</t>
   </si>
   <si>
     <t>The total number of lots for which contract(s) can be awarded to one tenderer.
-(WG Decision 12/12/2018)</t>
-  </si>
-  <si>
-    <t>Indicates whether the procurement documents are electronically available for unrestricted and full direct access, free of charge.
-(Pending to review by the WG)</t>
-  </si>
-  <si>
-    <t>The amount of bids received by the buyer from economic operators from other EU countries.
-(Pending to review by the WG)</t>
-  </si>
-  <si>
-    <t>The amount of applications to participate from economic operators.
-(Pending to review by the WG)</t>
-  </si>
-  <si>
-    <t>The amount of bids submitted by tenders.
-(Pending to review by the WG)</t>
-  </si>
-  <si>
-    <t>The winning tenderer has submited multiple additional proposals in response to a given set of requirements specified by the buyer in the procurement documents.
-(Pending to review by the WG)</t>
+(WG Approval 12/12/2018)</t>
+  </si>
+  <si>
+    <t>Indicates whether the procurement documents are electronically available for unrestricted and full direct access, free of charge.</t>
+  </si>
+  <si>
+    <t>The amount of bids received by the buyer from economic operators from other EU countries.</t>
+  </si>
+  <si>
+    <t>The amount of applications to participate from economic operators.</t>
+  </si>
+  <si>
+    <t>The amount of bids submitted by tenders.</t>
+  </si>
+  <si>
+    <t>The winning tenderer has submitted multiple additional proposals in response to a given set of requirements specified by the buyer in the procurement documents.</t>
   </si>
   <si>
     <t>The number of economic operators that requested the buyer to review any of its decisions (e.g. the technical specifications, award decision), as set out in Art. 1(5) of Directive 89/665/EEC and Directive 92/13/EEC.
-WG Approval 11/04/2019 15:58:37</t>
+WG Approval 11/04/2019</t>
   </si>
   <si>
     <t>The buyer emphasizes that this procurement is also suitable for small and medium enterprises (SMEs).
-WG Approval 11/04/2019 16:04:43</t>
+WG Approval 11/04/2019</t>
   </si>
   <si>
     <t>Any information not mentioned elsewhere.
-WG Approval 11/04/2019 16:58:18</t>
-  </si>
-  <si>
-    <t>In the case of a procurement procedure it includes options and renewals.
-(Pending to review by the WG)</t>
+WG Approval 11/04/2019</t>
+  </si>
+  <si>
+    <t>In the case of a procurement procedure it includes options and renewals.</t>
   </si>
   <si>
     <t>The highest amount which can be spent within a procurement over its whole duration.
-Additional Information: beware that the procurement can be organised based on different Techniques, e.g. Framework Agreements.
-(Pending to review by the WG)</t>
+Additional Information: beware that the procurement can be organised based on different Techniques, e.g. Framework Agreements.</t>
   </si>
   <si>
     <t>The description of the system used for calculating the estimated value of procurement.
 Additional information: e.g. the method used to calculate the estimated value of a concession and any other relevant information.
-WG Approval 25/04/2019 17:01:13</t>
+WG Approval 25/04/2019</t>
   </si>
   <si>
     <t>The buyer reserves the right (not an obligation) for additional purchases from the contractor (while the contract is valid).
 WG Approval 09/04/2019 14:45:05
 The old definition we had in ePO reads as follows (and never was approved by the WG:
-"Statement by the Procuring Entity about whether it may apply modifications to the procurement procedure that would alter the overall nature of the contract or the framework agreement."
-(Pending to review by the WG)</t>
+"Statement by the Procuring Entity about whether it may apply modifications to the procurement procedure that would alter the overall nature of the contract or the framework agreement."</t>
   </si>
   <si>
     <t>The CPV establishes a single classification system for public procurement aimed at standardising the references used by procuring entities to describe the purpose of procurement contracts and procurement projects.
@@ -1649,24 +1618,24 @@
   </si>
   <si>
     <t>ISO 15000 ebXML CCTS QuantityType uses the attribute "unitCode" to specify what the quantity is about.
-Example: 3 months; 131 printers; 1,000 tones; etc.
-(Pending to review by the WG)</t>
-  </si>
-  <si>
-    <t>The nature of the contract, which corresponds to the main subject of the contract.
-(Pending to review by the WG))</t>
-  </si>
-  <si>
-    <t>The common classification of territorial units for statistics.
-(Pending to review by the WG)</t>
+Example: 3 months; 131 printers; 1,000 tones; etc.</t>
+  </si>
+  <si>
+    <t>The nature of the contract, which corresponds to the main subject of the contract.</t>
+  </si>
+  <si>
+    <t>The common classification of territorial units for statistics.</t>
   </si>
   <si>
     <t>The motivation and details about additional purchases that the buyer may undertake while the contract is valid.
-WG Approval 09/04/2019 14:48:06</t>
+WG Approval 09/04/2019</t>
+  </si>
+  <si>
+    <t>The estimated proportion foreseen to be subcontracted.</t>
   </si>
   <si>
     <t>Whether subcontracting will be used or not (or not known yet).
-WG Approved 08/05/2019</t>
+WG Approval 08/05/2019</t>
   </si>
   <si>
     <t>The estimated value of the part of the contract to be subcontracted.
@@ -1674,7 +1643,7 @@
   </si>
   <si>
     <t>The estimated share of the subcontracting can be calculated.
-WG Approval 07/05/2019 16:06:30</t>
+WG Approval 07/05/2019</t>
   </si>
   <si>
     <t>The estimated value of the subcontracting can be calculated.
@@ -1691,7 +1660,7 @@
   </si>
   <si>
     <t>Self-explanatory text about a concept.
-WG Approved 08/05/2019</t>
+WG Approval 08/05/2019</t>
   </si>
   <si>
     <t>The maximum proportion of something to be distributed.
@@ -1707,11 +1676,13 @@
     <t>List of Subcontractors and the subject matter they cover are required.
 Additional Information: 
 The tenderer will ned to supply this information in the tender.
-WG Approval 28/02/2019 16:41:59</t>
-  </si>
-  <si>
-    <t>The period during which tenders submitted for this procurement procedure must remain valid.
-(Pending to review by the WG)</t>
+WG Approval 28/02/2019</t>
+  </si>
+  <si>
+    <t>The deadline for submitting Tenders.</t>
+  </si>
+  <si>
+    <t>The period during which tenders submitted for this procurement procedure must remain valid.</t>
   </si>
   <si>
     <t>Including the financial modality and request for commitment reserved to be used in case of default.
@@ -1734,29 +1705,26 @@
 Additional Information: 
 Signature can be defined as "data in electronic form which is attached to or logically associated with other data in electronic form and which is used by the signatory to sign. 
 For more details on the meaning and uses of electronic signature you may consult different authoritative sources, a relevant one being for instance the Regulation (EU) 910/2014 on electronic identification and trust services for electronic transactions in the internal market.
-WG Approval 12/03/2019 15:46:34</t>
+WG Approval 12/03/2019</t>
   </si>
   <si>
     <t>Procurement criteria for persons with disabilities applied.
-WG Approval 05/03/2019 15:54:49</t>
+WG Approval 05/03/2019</t>
   </si>
   <si>
     <t>Reason for not applying accessibility criteria.
-WG Approval 05/03/2019 15:52:31</t>
-  </si>
-  <si>
-    <t>Transmission of tenders is possible by electronic means of communication. 
-(Pending to review by the WG)</t>
-  </si>
-  <si>
-    <t>Basis for physical submission of tenders.
-(Pending to review by the WG)</t>
+WG Approval 05/03/2019</t>
+  </si>
+  <si>
+    <t>Transmission of tenders is possible by electronic means of communication.</t>
+  </si>
+  <si>
+    <t>Basis for physical submission of tenders.</t>
   </si>
   <si>
     <t>The value of the tender is needed for awarding purposes.
 max(Tender.Value) where Tender.eligible is True for a given Lot.
-Related to BT-710 and BT-711.
-TO BE DISCUSSED FURTHER</t>
+Related to BT-710 and BT-711.</t>
   </si>
   <si>
     <t>If there's no first stage then there is only a final stage.</t>
@@ -1764,7 +1732,7 @@
   <si>
     <t>The position of the winner, i.e. whether the economic operator ended up first, second, third, etc.
 Additional information: This is specially the case of design contests, some framework agreements with multiple winners (e.g. cascades) or innovation partnerships.
-WG Approval 25/04/2019 16:28:00</t>
+WG Approval 25/04/2019</t>
   </si>
   <si>
     <t>The date on which this period begins.</t>
@@ -1827,8 +1795,11 @@
     <t>xsd:string</t>
   </si>
   <si>
-    <t>The execution of the contract is restricted to the framework of sheltered employment programmes.
-Pending of approval</t>
+    <t>An announcement of the award or non-award of a contract by a procuring entity.
+(WG approval 27/03/2019)</t>
+  </si>
+  <si>
+    <t>The execution of the contract is restricted to the framework of sheltered employment programmers.</t>
   </si>
   <si>
     <t>Identifies the criterion unambiguously and uniquely across all  procurement procedures.</t>
@@ -1841,31 +1812,10 @@
 reviewed on 23-01-2019)</t>
   </si>
   <si>
-    <t>Describes the object of the procurement and the properties of the procedure.
-(Pending to review by the WG)</t>
-  </si>
-  <si>
     <t>Active and dynamic files representing information.
-(Pending to review by the WG)
 This other definition comes from ISA2, we want to propose it for discussion to the WG: 
 The definition o eBusiness Document may be useful to refine our ePO definition. It goes as follows:
 "a set of interrelated Business Information representing the business facts, data, or opinions, in any medium or form, including textual, numerical, graphic, cartographic, narrative, or audio-visual forms that the capability exchanges with other capabilities to support the execution of value streams."</t>
-  </si>
-  <si>
-    <t>Explanation about why the choice of an accelerated procedure is lawful.
-(Pending to review by the WG)</t>
-  </si>
-  <si>
-    <t>The estimated proportion foreseen to be subcontracted.
-(Pending to review by the WG)</t>
-  </si>
-  <si>
-    <t>The deadline for submitting Tenders.
-(Pending to review by the WG)</t>
-  </si>
-  <si>
-    <t>The tenderer to whom the contract is awarded.
-(WG approval 20/11/2018)</t>
   </si>
 </sst>
 </file>
@@ -2276,13 +2226,13 @@
   <dimension ref="A1:E340"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C270" sqref="C270"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="81.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="48.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="81.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
@@ -2310,9 +2260,7 @@
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>154</v>
-      </c>
+      <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -2330,7 +2278,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -2341,7 +2289,7 @@
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -2358,7 +2306,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
@@ -2373,7 +2321,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -2385,10 +2333,10 @@
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -2403,7 +2351,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
@@ -2415,10 +2363,10 @@
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -2433,7 +2381,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
@@ -2445,10 +2393,10 @@
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
@@ -2460,10 +2408,10 @@
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
@@ -2478,7 +2426,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>16</v>
       </c>
@@ -2493,7 +2441,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>16</v>
       </c>
@@ -2508,7 +2456,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
@@ -2615,7 +2563,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>20</v>
       </c>
@@ -2626,7 +2574,7 @@
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>21</v>
       </c>
@@ -2637,7 +2585,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>22</v>
       </c>
@@ -2651,10 +2599,10 @@
         <v>425</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>22</v>
       </c>
@@ -2668,10 +2616,10 @@
         <v>426</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>22</v>
       </c>
@@ -2685,10 +2633,10 @@
         <v>427</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>23</v>
       </c>
@@ -2813,23 +2761,23 @@
         <v>195</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>129</v>
+        <v>533</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
     </row>
-    <row r="38" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>178</v>
@@ -2839,12 +2787,12 @@
         <v>198</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>208</v>
@@ -2854,12 +2802,12 @@
         <v>198</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>208</v>
@@ -2869,12 +2817,12 @@
         <v>194</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>225</v>
@@ -2884,12 +2832,12 @@
         <v>197</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>226</v>
@@ -2910,12 +2858,12 @@
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
     </row>
-    <row r="44" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>227</v>
@@ -2924,15 +2872,15 @@
         <v>431</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>228</v>
@@ -2949,7 +2897,7 @@
         <v>30</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>229</v>
@@ -2961,12 +2909,12 @@
         <v>198</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>230</v>
@@ -2978,12 +2926,12 @@
         <v>197</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>231</v>
@@ -2995,12 +2943,12 @@
         <v>197</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>232</v>
@@ -3010,12 +2958,12 @@
         <v>197</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>233</v>
@@ -3032,7 +2980,7 @@
         <v>30</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>234</v>
@@ -3044,12 +2992,12 @@
         <v>197</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>235</v>
@@ -3059,12 +3007,12 @@
         <v>197</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>236</v>
@@ -3081,7 +3029,7 @@
         <v>30</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>237</v>
@@ -3093,29 +3041,29 @@
         <v>198</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>238</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>531</v>
+        <v>534</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>239</v>
@@ -3185,7 +3133,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>5</v>
       </c>
@@ -3196,13 +3144,13 @@
         <v>176</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>5</v>
       </c>
@@ -3219,7 +3167,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>5</v>
       </c>
@@ -3236,7 +3184,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>5</v>
       </c>
@@ -3264,13 +3212,13 @@
         <v>180</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>533</v>
+        <v>536</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>5</v>
       </c>
@@ -3285,7 +3233,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>5</v>
       </c>
@@ -3300,7 +3248,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>5</v>
       </c>
@@ -3432,12 +3380,12 @@
         <v>194</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>534</v>
+        <v>132</v>
       </c>
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>
@@ -3453,7 +3401,7 @@
       </c>
       <c r="D77" s="2"/>
       <c r="E77" s="2" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -3533,30 +3481,30 @@
       </c>
       <c r="D83" s="2"/>
       <c r="E83" s="2" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" ht="210" x14ac:dyDescent="0.25">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="150" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>176</v>
       </c>
       <c r="D84" s="2"/>
       <c r="E84" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" ht="210" x14ac:dyDescent="0.25">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="150" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>248</v>
@@ -3565,15 +3513,15 @@
         <v>442</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" ht="210" x14ac:dyDescent="0.25">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="150" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>249</v>
@@ -3582,15 +3530,15 @@
         <v>443</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" ht="210" x14ac:dyDescent="0.25">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="150" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="C87" s="2" t="s">
         <v>250</v>
@@ -3611,7 +3559,7 @@
       <c r="D88" s="2"/>
       <c r="E88" s="2"/>
     </row>
-    <row r="89" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>36</v>
       </c>
@@ -3628,7 +3576,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>36</v>
       </c>
@@ -3668,10 +3616,10 @@
         <v>446</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>38</v>
       </c>
@@ -3682,7 +3630,7 @@
       <c r="D93" s="2"/>
       <c r="E93" s="2"/>
     </row>
-    <row r="94" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>39</v>
       </c>
@@ -3693,7 +3641,7 @@
       <c r="D94" s="2"/>
       <c r="E94" s="2"/>
     </row>
-    <row r="95" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>40</v>
       </c>
@@ -3708,7 +3656,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>40</v>
       </c>
@@ -3725,7 +3673,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>40</v>
       </c>
@@ -3740,7 +3688,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>40</v>
       </c>
@@ -3757,7 +3705,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>40</v>
       </c>
@@ -3772,7 +3720,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>41</v>
       </c>
@@ -3789,7 +3737,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="101" spans="1:5" ht="270" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" ht="210" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>42</v>
       </c>
@@ -3806,7 +3754,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="102" spans="1:5" ht="270" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" ht="210" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>42</v>
       </c>
@@ -3821,7 +3769,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="103" spans="1:5" ht="270" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" ht="210" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>42</v>
       </c>
@@ -3864,7 +3812,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>44</v>
       </c>
@@ -3875,7 +3823,7 @@
       <c r="D106" s="2"/>
       <c r="E106" s="2"/>
     </row>
-    <row r="107" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>45</v>
       </c>
@@ -3899,7 +3847,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="109" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>47</v>
       </c>
@@ -3916,7 +3864,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="110" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>47</v>
       </c>
@@ -3928,10 +3876,10 @@
       </c>
       <c r="D110" s="2"/>
       <c r="E110" s="2" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>47</v>
       </c>
@@ -3948,7 +3896,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="112" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>47</v>
       </c>
@@ -3978,7 +3926,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="114" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>49</v>
       </c>
@@ -4012,7 +3960,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="116" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>49</v>
       </c>
@@ -4022,14 +3970,12 @@
       <c r="C116" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="D116" s="2" t="s">
-        <v>455</v>
-      </c>
+      <c r="D116" s="2"/>
       <c r="E116" s="2" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>49</v>
       </c>
@@ -4041,10 +3987,10 @@
       </c>
       <c r="D117" s="2"/>
       <c r="E117" s="2" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>49</v>
       </c>
@@ -4056,7 +4002,7 @@
       </c>
       <c r="D118" s="2"/>
       <c r="E118" s="2" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -4072,9 +4018,7 @@
       <c r="A120" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B120" s="2" t="s">
-        <v>154</v>
-      </c>
+      <c r="B120" s="2"/>
       <c r="C120" s="2" t="s">
         <v>176</v>
       </c>
@@ -4087,9 +4031,7 @@
       <c r="A121" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B121" s="2" t="s">
-        <v>154</v>
-      </c>
+      <c r="B121" s="2"/>
       <c r="C121" s="2" t="s">
         <v>177</v>
       </c>
@@ -4102,9 +4044,7 @@
       <c r="A122" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B122" s="2" t="s">
-        <v>154</v>
-      </c>
+      <c r="B122" s="2"/>
       <c r="C122" s="2" t="s">
         <v>178</v>
       </c>
@@ -4119,9 +4059,7 @@
       <c r="A123" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B123" s="2" t="s">
-        <v>154</v>
-      </c>
+      <c r="B123" s="2"/>
       <c r="C123" s="2" t="s">
         <v>185</v>
       </c>
@@ -4130,7 +4068,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="124" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>51</v>
       </c>
@@ -4257,7 +4195,7 @@
         <v>107</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E132" s="2" t="s">
         <v>194</v>
@@ -4267,14 +4205,12 @@
       <c r="A133" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B133" s="2" t="s">
-        <v>154</v>
-      </c>
+      <c r="B133" s="2"/>
       <c r="C133" s="2"/>
       <c r="D133" s="2"/>
       <c r="E133" s="2"/>
     </row>
-    <row r="134" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>54</v>
       </c>
@@ -4285,7 +4221,7 @@
       <c r="D134" s="2"/>
       <c r="E134" s="2"/>
     </row>
-    <row r="135" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>55</v>
       </c>
@@ -4300,7 +4236,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="136" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>55</v>
       </c>
@@ -4311,13 +4247,13 @@
         <v>280</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="E136" s="2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="137" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>55</v>
       </c>
@@ -4328,13 +4264,13 @@
         <v>281</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="E137" s="2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="138" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>55</v>
       </c>
@@ -4345,13 +4281,13 @@
         <v>282</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="E138" s="2" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="139" spans="1:5" ht="225" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" ht="180" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>56</v>
       </c>
@@ -4366,7 +4302,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="140" spans="1:5" ht="225" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" ht="180" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>56</v>
       </c>
@@ -4376,14 +4312,12 @@
       <c r="C140" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="D140" s="2" t="s">
-        <v>154</v>
-      </c>
+      <c r="D140" s="2"/>
       <c r="E140" s="2" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="141" spans="1:5" ht="225" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" ht="180" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>56</v>
       </c>
@@ -4489,9 +4423,7 @@
       <c r="A149" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B149" s="2" t="s">
-        <v>154</v>
-      </c>
+      <c r="B149" s="2"/>
       <c r="C149" s="2"/>
       <c r="D149" s="2"/>
       <c r="E149" s="2"/>
@@ -4506,7 +4438,7 @@
       </c>
       <c r="D150" s="2"/>
       <c r="E150" s="2" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
@@ -4563,7 +4495,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="155" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
         <v>9</v>
       </c>
@@ -4578,7 +4510,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="156" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
         <v>9</v>
       </c>
@@ -4612,7 +4544,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="158" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
         <v>9</v>
       </c>
@@ -4627,7 +4559,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="159" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
         <v>9</v>
       </c>
@@ -4642,7 +4574,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="160" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
         <v>9</v>
       </c>
@@ -4680,7 +4612,7 @@
       </c>
       <c r="D162" s="2"/>
       <c r="E162" s="2" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
@@ -4693,7 +4625,7 @@
       </c>
       <c r="D163" s="2"/>
       <c r="E163" s="2" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
@@ -4719,7 +4651,7 @@
       </c>
       <c r="D165" s="2"/>
       <c r="E165" s="2" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
@@ -4732,7 +4664,7 @@
       </c>
       <c r="D166" s="2"/>
       <c r="E166" s="2" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
@@ -4758,10 +4690,10 @@
       </c>
       <c r="D168" s="2"/>
       <c r="E168" s="2" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="169" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
         <v>61</v>
       </c>
@@ -4778,7 +4710,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="170" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
         <v>61</v>
       </c>
@@ -4793,7 +4725,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="171" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
         <v>61</v>
       </c>
@@ -4808,7 +4740,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="172" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
         <v>61</v>
       </c>
@@ -4823,7 +4755,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="173" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
         <v>61</v>
       </c>
@@ -4834,13 +4766,13 @@
         <v>290</v>
       </c>
       <c r="D173" s="2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="E173" s="2" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="174" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
         <v>61</v>
       </c>
@@ -4855,7 +4787,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="175" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
         <v>61</v>
       </c>
@@ -4870,7 +4802,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="176" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
         <v>62</v>
       </c>
@@ -4885,7 +4817,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="177" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
         <v>62</v>
       </c>
@@ -4902,7 +4834,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="178" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
         <v>62</v>
       </c>
@@ -4917,7 +4849,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="179" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
         <v>63</v>
       </c>
@@ -4932,7 +4864,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="180" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
         <v>63</v>
       </c>
@@ -4947,7 +4879,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="181" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
         <v>63</v>
       </c>
@@ -4962,7 +4894,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="182" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
         <v>63</v>
       </c>
@@ -4977,7 +4909,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="183" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
         <v>64</v>
       </c>
@@ -4988,13 +4920,13 @@
         <v>295</v>
       </c>
       <c r="D183" s="2" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="E183" s="2" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="184" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
         <v>64</v>
       </c>
@@ -5009,7 +4941,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="185" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
         <v>65</v>
       </c>
@@ -5033,10 +4965,10 @@
         <v>298</v>
       </c>
       <c r="D186" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E186" s="2" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
     </row>
     <row r="187" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -5048,13 +4980,13 @@
         <v>299</v>
       </c>
       <c r="D187" s="2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="E187" s="2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="188" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
         <v>104</v>
       </c>
@@ -5076,10 +5008,10 @@
         <v>385</v>
       </c>
       <c r="D189" s="2" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="E189" s="2" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
     </row>
     <row r="190" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -5093,10 +5025,10 @@
         <v>386</v>
       </c>
       <c r="D190" s="2" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="E190" s="2" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
     </row>
     <row r="191" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -5110,10 +5042,10 @@
         <v>387</v>
       </c>
       <c r="D191" s="2" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="E191" s="2" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
     </row>
     <row r="192" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -5127,10 +5059,10 @@
         <v>388</v>
       </c>
       <c r="D192" s="2" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="E192" s="2" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
     </row>
     <row r="193" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -5144,10 +5076,10 @@
         <v>389</v>
       </c>
       <c r="D193" s="2" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="E193" s="2" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
     </row>
     <row r="194" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -5161,10 +5093,10 @@
         <v>390</v>
       </c>
       <c r="D194" s="2" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="E194" s="2" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
     </row>
     <row r="195" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -5178,10 +5110,10 @@
         <v>391</v>
       </c>
       <c r="D195" s="2" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="E195" s="2" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
@@ -5505,19 +5437,17 @@
       <c r="A221" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B221" s="2" t="s">
-        <v>154</v>
-      </c>
+      <c r="B221" s="2"/>
       <c r="C221" s="2"/>
       <c r="D221" s="2"/>
       <c r="E221" s="2"/>
     </row>
-    <row r="222" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C222" s="2"/>
       <c r="D222" s="2"/>
@@ -5528,13 +5458,13 @@
         <v>70</v>
       </c>
       <c r="B223" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C223" s="2" t="s">
         <v>300</v>
       </c>
       <c r="D223" s="2" t="s">
-        <v>536</v>
+        <v>463</v>
       </c>
       <c r="E223" s="2" t="s">
         <v>198</v>
@@ -5545,7 +5475,7 @@
         <v>70</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C224" s="2" t="s">
         <v>301</v>
@@ -5562,7 +5492,7 @@
         <v>70</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C225" s="2" t="s">
         <v>302</v>
@@ -5577,7 +5507,7 @@
         <v>70</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C226" s="2" t="s">
         <v>303</v>
@@ -5594,7 +5524,7 @@
         <v>70</v>
       </c>
       <c r="B227" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C227" s="2" t="s">
         <v>304</v>
@@ -5611,14 +5541,12 @@
         <v>70</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C228" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="D228" s="2" t="s">
-        <v>154</v>
-      </c>
+      <c r="D228" s="2"/>
       <c r="E228" s="2" t="s">
         <v>194</v>
       </c>
@@ -5628,14 +5556,12 @@
         <v>70</v>
       </c>
       <c r="B229" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C229" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="D229" s="2" t="s">
-        <v>154</v>
-      </c>
+      <c r="D229" s="2"/>
       <c r="E229" s="2" t="s">
         <v>194</v>
       </c>
@@ -5645,7 +5571,7 @@
         <v>70</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C230" s="2" t="s">
         <v>191</v>
@@ -5660,7 +5586,7 @@
         <v>70</v>
       </c>
       <c r="B231" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C231" s="2" t="s">
         <v>178</v>
@@ -5677,7 +5603,7 @@
         <v>70</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C232" s="2" t="s">
         <v>186</v>
@@ -5692,7 +5618,7 @@
         <v>70</v>
       </c>
       <c r="B233" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C233" s="2" t="s">
         <v>307</v>
@@ -5707,7 +5633,7 @@
         <v>70</v>
       </c>
       <c r="B234" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C234" s="2" t="s">
         <v>308</v>
@@ -5716,7 +5642,7 @@
         <v>467</v>
       </c>
       <c r="E234" s="2" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
     </row>
     <row r="235" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -5724,22 +5650,22 @@
         <v>70</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C235" s="2" t="s">
         <v>309</v>
       </c>
       <c r="D235" s="2"/>
       <c r="E235" s="2" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="236" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A236" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C236" s="2" t="s">
         <v>310</v>
@@ -5751,12 +5677,12 @@
         <v>197</v>
       </c>
     </row>
-    <row r="237" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A237" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C237" s="2" t="s">
         <v>254</v>
@@ -5766,12 +5692,12 @@
         <v>195</v>
       </c>
     </row>
-    <row r="238" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A238" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B238" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C238" s="2" t="s">
         <v>311</v>
@@ -5783,29 +5709,27 @@
         <v>195</v>
       </c>
     </row>
-    <row r="239" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A239" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C239" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="D239" s="2" t="s">
-        <v>154</v>
-      </c>
+      <c r="D239" s="2"/>
       <c r="E239" s="2" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="240" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A240" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C240" s="2" t="s">
         <v>313</v>
@@ -5817,12 +5741,12 @@
         <v>195</v>
       </c>
     </row>
-    <row r="241" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A241" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B241" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C241" s="2" t="s">
         <v>314</v>
@@ -5831,16 +5755,14 @@
         <v>471</v>
       </c>
       <c r="E241" s="2" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B242" s="2" t="s">
-        <v>154</v>
-      </c>
+      <c r="B242" s="2"/>
       <c r="C242" s="2"/>
       <c r="D242" s="2"/>
       <c r="E242" s="2"/>
@@ -5849,9 +5771,7 @@
       <c r="A243" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B243" s="2" t="s">
-        <v>154</v>
-      </c>
+      <c r="B243" s="2"/>
       <c r="C243" s="2"/>
       <c r="D243" s="2"/>
       <c r="E243" s="2"/>
@@ -5860,19 +5780,17 @@
       <c r="A244" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B244" s="2" t="s">
-        <v>154</v>
-      </c>
+      <c r="B244" s="2"/>
       <c r="C244" s="2"/>
       <c r="D244" s="2"/>
       <c r="E244" s="2"/>
     </row>
-    <row r="245" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A245" s="2" t="s">
         <v>75</v>
       </c>
       <c r="B245" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C245" s="2" t="s">
         <v>315</v>
@@ -5884,12 +5802,12 @@
         <v>197</v>
       </c>
     </row>
-    <row r="246" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A246" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B246" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C246" s="2" t="s">
         <v>316</v>
@@ -5898,15 +5816,15 @@
         <v>473</v>
       </c>
       <c r="E246" s="2" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="247" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A247" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B247" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C247" s="2" t="s">
         <v>317</v>
@@ -5915,15 +5833,15 @@
         <v>474</v>
       </c>
       <c r="E247" s="2" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="248" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A248" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C248" s="2" t="s">
         <v>318</v>
@@ -5932,15 +5850,15 @@
         <v>475</v>
       </c>
       <c r="E248" s="2" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="249" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A249" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C249" s="2" t="s">
         <v>319</v>
@@ -5949,22 +5867,22 @@
         <v>476</v>
       </c>
       <c r="E249" s="2" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="250" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A250" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C250" s="2" t="s">
         <v>320</v>
       </c>
       <c r="D250" s="2"/>
       <c r="E250" s="2" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
     </row>
     <row r="251" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -5972,7 +5890,7 @@
         <v>76</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C251" s="2" t="s">
         <v>321</v>
@@ -5981,15 +5899,15 @@
         <v>477</v>
       </c>
       <c r="E251" s="2" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="252" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A252" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B252" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C252" s="2" t="s">
         <v>322</v>
@@ -6001,12 +5919,12 @@
         <v>197</v>
       </c>
     </row>
-    <row r="253" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A253" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B253" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C253" s="2" t="s">
         <v>261</v>
@@ -6032,7 +5950,7 @@
         <v>78</v>
       </c>
       <c r="B255" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C255" s="2" t="s">
         <v>323</v>
@@ -6049,14 +5967,12 @@
         <v>78</v>
       </c>
       <c r="B256" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C256" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="D256" s="2" t="s">
-        <v>154</v>
-      </c>
+      <c r="D256" s="2"/>
       <c r="E256" s="2" t="s">
         <v>192</v>
       </c>
@@ -6066,7 +5982,7 @@
         <v>78</v>
       </c>
       <c r="B257" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C257" s="2" t="s">
         <v>325</v>
@@ -6081,24 +5997,22 @@
         <v>78</v>
       </c>
       <c r="B258" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C258" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="D258" s="2" t="s">
-        <v>154</v>
-      </c>
+      <c r="D258" s="2"/>
       <c r="E258" s="2" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="259" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A259" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B259" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C259" s="2" t="s">
         <v>327</v>
@@ -6115,7 +6029,7 @@
         <v>78</v>
       </c>
       <c r="B260" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C260" s="2" t="s">
         <v>328</v>
@@ -6178,19 +6092,17 @@
       <c r="A264" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B264" s="2" t="s">
-        <v>154</v>
-      </c>
+      <c r="B264" s="2"/>
       <c r="C264" s="2"/>
       <c r="D264" s="2"/>
       <c r="E264" s="2"/>
     </row>
-    <row r="265" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A265" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B265" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C265" s="2" t="s">
         <v>329</v>
@@ -6202,12 +6114,12 @@
         <v>197</v>
       </c>
     </row>
-    <row r="266" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A266" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B266" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C266" s="2" t="s">
         <v>330</v>
@@ -6219,12 +6131,12 @@
         <v>194</v>
       </c>
     </row>
-    <row r="267" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A267" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B267" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C267" s="2" t="s">
         <v>331</v>
@@ -6236,12 +6148,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="268" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A268" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B268" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C268" s="2" t="s">
         <v>332</v>
@@ -6253,29 +6165,27 @@
         <v>194</v>
       </c>
     </row>
-    <row r="269" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A269" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B269" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C269" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="D269" s="2" t="s">
-        <v>154</v>
-      </c>
+      <c r="D269" s="2"/>
       <c r="E269" s="2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="270" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A270" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B270" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C270" s="2" t="s">
         <v>334</v>
@@ -6287,12 +6197,12 @@
         <v>194</v>
       </c>
     </row>
-    <row r="271" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A271" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B271" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C271" s="2" t="s">
         <v>335</v>
@@ -6302,12 +6212,12 @@
         <v>194</v>
       </c>
     </row>
-    <row r="272" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A272" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B272" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C272" s="2" t="s">
         <v>336</v>
@@ -6323,51 +6233,47 @@
       <c r="A273" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B273" s="2" t="s">
-        <v>154</v>
-      </c>
+      <c r="B273" s="2"/>
       <c r="C273" s="2"/>
       <c r="D273" s="2"/>
       <c r="E273" s="2"/>
     </row>
-    <row r="274" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A274" s="2" t="s">
         <v>82</v>
       </c>
       <c r="B274" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C274" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="D274" s="2" t="s">
-        <v>154</v>
-      </c>
+      <c r="D274" s="2"/>
       <c r="E274" s="2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="275" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A275" s="2" t="s">
         <v>82</v>
       </c>
       <c r="B275" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C275" s="2" t="s">
         <v>338</v>
       </c>
       <c r="D275" s="2"/>
       <c r="E275" s="2" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="276" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="276" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A276" s="2" t="s">
         <v>82</v>
       </c>
       <c r="B276" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C276" s="2" t="s">
         <v>339</v>
@@ -6377,12 +6283,12 @@
         <v>198</v>
       </c>
     </row>
-    <row r="277" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A277" s="2" t="s">
         <v>83</v>
       </c>
       <c r="B277" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C277" s="2" t="s">
         <v>340</v>
@@ -6392,12 +6298,12 @@
         <v>195</v>
       </c>
     </row>
-    <row r="278" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A278" s="2" t="s">
         <v>83</v>
       </c>
       <c r="B278" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C278" s="2" t="s">
         <v>178</v>
@@ -6414,7 +6320,7 @@
         <v>84</v>
       </c>
       <c r="B279" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C279" s="2" t="s">
         <v>200</v>
@@ -6429,23 +6335,21 @@
         <v>84</v>
       </c>
       <c r="B280" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C280" s="2" t="s">
         <v>201</v>
       </c>
       <c r="D280" s="2"/>
       <c r="E280" s="2" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
     </row>
     <row r="281" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A281" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B281" s="2" t="s">
-        <v>154</v>
-      </c>
+      <c r="B281" s="2"/>
       <c r="C281" s="2"/>
       <c r="D281" s="2"/>
       <c r="E281" s="2"/>
@@ -6472,12 +6376,12 @@
         <v>198</v>
       </c>
     </row>
-    <row r="284" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A284" s="2" t="s">
         <v>87</v>
       </c>
       <c r="B284" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C284" s="2" t="s">
         <v>341</v>
@@ -6494,7 +6398,7 @@
         <v>88</v>
       </c>
       <c r="B285" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C285" s="2" t="s">
         <v>178</v>
@@ -6511,16 +6415,16 @@
         <v>88</v>
       </c>
       <c r="B286" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C286" s="2" t="s">
         <v>342</v>
       </c>
       <c r="D286" s="2" t="s">
-        <v>537</v>
+        <v>489</v>
       </c>
       <c r="E286" s="2" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
     </row>
     <row r="287" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -6528,13 +6432,13 @@
         <v>88</v>
       </c>
       <c r="B287" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C287" s="2" t="s">
         <v>343</v>
       </c>
       <c r="D287" s="2" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="E287" s="2" t="s">
         <v>194</v>
@@ -6545,13 +6449,13 @@
         <v>88</v>
       </c>
       <c r="B288" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C288" s="2" t="s">
         <v>344</v>
       </c>
       <c r="D288" s="2" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="E288" s="2" t="s">
         <v>192</v>
@@ -6562,13 +6466,13 @@
         <v>88</v>
       </c>
       <c r="B289" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C289" s="2" t="s">
         <v>345</v>
       </c>
       <c r="D289" s="2" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="E289" s="2" t="s">
         <v>197</v>
@@ -6579,13 +6483,13 @@
         <v>88</v>
       </c>
       <c r="B290" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C290" s="2" t="s">
         <v>346</v>
       </c>
       <c r="D290" s="2" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="E290" s="2" t="s">
         <v>197</v>
@@ -6596,13 +6500,13 @@
         <v>88</v>
       </c>
       <c r="B291" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C291" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D291" s="2" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="E291" s="2" t="s">
         <v>192</v>
@@ -6613,30 +6517,30 @@
         <v>88</v>
       </c>
       <c r="B292" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C292" s="2" t="s">
         <v>347</v>
       </c>
       <c r="D292" s="2" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="E292" s="2" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="293" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="293" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A293" s="2" t="s">
         <v>89</v>
       </c>
       <c r="B293" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C293" s="2" t="s">
         <v>178</v>
       </c>
       <c r="D293" s="2" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="E293" s="2" t="s">
         <v>198</v>
@@ -6647,16 +6551,16 @@
         <v>89</v>
       </c>
       <c r="B294" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C294" s="2" t="s">
         <v>348</v>
       </c>
       <c r="D294" s="2" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="E294" s="2" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
     </row>
     <row r="295" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -6664,16 +6568,16 @@
         <v>89</v>
       </c>
       <c r="B295" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C295" s="2" t="s">
         <v>349</v>
       </c>
       <c r="D295" s="2" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="E295" s="2" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
     </row>
     <row r="296" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -6681,24 +6585,24 @@
         <v>89</v>
       </c>
       <c r="B296" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C296" s="2" t="s">
         <v>350</v>
       </c>
       <c r="D296" s="2" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="E296" s="2" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="297" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A297" s="2" t="s">
         <v>89</v>
       </c>
       <c r="B297" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C297" s="2" t="s">
         <v>351</v>
@@ -6708,12 +6612,12 @@
         <v>198</v>
       </c>
     </row>
-    <row r="298" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A298" s="2" t="s">
         <v>89</v>
       </c>
       <c r="B298" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C298" s="2" t="s">
         <v>352</v>
@@ -6723,12 +6627,12 @@
         <v>197</v>
       </c>
     </row>
-    <row r="299" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A299" s="2" t="s">
         <v>89</v>
       </c>
       <c r="B299" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C299" s="2" t="s">
         <v>353</v>
@@ -6738,12 +6642,12 @@
         <v>194</v>
       </c>
     </row>
-    <row r="300" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A300" s="2" t="s">
         <v>89</v>
       </c>
       <c r="B300" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C300" s="2" t="s">
         <v>354</v>
@@ -6758,7 +6662,7 @@
         <v>90</v>
       </c>
       <c r="B301" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C301" s="2" t="s">
         <v>355</v>
@@ -6773,33 +6677,33 @@
         <v>90</v>
       </c>
       <c r="B302" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C302" s="2" t="s">
         <v>356</v>
       </c>
       <c r="D302" s="2" t="s">
-        <v>538</v>
+        <v>500</v>
       </c>
       <c r="E302" s="2" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="303" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="303" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A303" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B303" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C303" s="2" t="s">
         <v>357</v>
       </c>
       <c r="D303" s="2" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="E303" s="2" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
     </row>
     <row r="304" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -6807,7 +6711,7 @@
         <v>90</v>
       </c>
       <c r="B304" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C304" s="2" t="s">
         <v>297</v>
@@ -6822,13 +6726,13 @@
         <v>90</v>
       </c>
       <c r="B305" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C305" s="2" t="s">
         <v>358</v>
       </c>
       <c r="D305" s="2" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="E305" s="2" t="s">
         <v>197</v>
@@ -6839,13 +6743,13 @@
         <v>90</v>
       </c>
       <c r="B306" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C306" s="2" t="s">
         <v>359</v>
       </c>
       <c r="D306" s="2" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="E306" s="2" t="s">
         <v>198</v>
@@ -6856,7 +6760,7 @@
         <v>90</v>
       </c>
       <c r="B307" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C307" s="2" t="s">
         <v>39</v>
@@ -6871,13 +6775,13 @@
         <v>90</v>
       </c>
       <c r="B308" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C308" s="2" t="s">
         <v>360</v>
       </c>
       <c r="D308" s="2" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="E308" s="2" t="s">
         <v>194</v>
@@ -6888,7 +6792,7 @@
         <v>90</v>
       </c>
       <c r="B309" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C309" s="2" t="s">
         <v>361</v>
@@ -6903,7 +6807,7 @@
         <v>90</v>
       </c>
       <c r="B310" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C310" s="2" t="s">
         <v>362</v>
@@ -6918,13 +6822,13 @@
         <v>90</v>
       </c>
       <c r="B311" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C311" s="2" t="s">
         <v>363</v>
       </c>
       <c r="D311" s="2" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="E311" s="2" t="s">
         <v>197</v>
@@ -6934,14 +6838,12 @@
       <c r="A312" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B312" s="2" t="s">
-        <v>154</v>
-      </c>
+      <c r="B312" s="2"/>
       <c r="C312" s="2" t="s">
         <v>364</v>
       </c>
       <c r="D312" s="2" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="E312" s="2" t="s">
         <v>194</v>
@@ -6951,14 +6853,12 @@
       <c r="A313" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B313" s="2" t="s">
-        <v>154</v>
-      </c>
+      <c r="B313" s="2"/>
       <c r="C313" s="2" t="s">
         <v>365</v>
       </c>
       <c r="D313" s="2" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="E313" s="2" t="s">
         <v>198</v>
@@ -6968,19 +6868,17 @@
       <c r="A314" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B314" s="2" t="s">
-        <v>154</v>
-      </c>
+      <c r="B314" s="2"/>
       <c r="C314" s="2"/>
       <c r="D314" s="2"/>
       <c r="E314" s="2"/>
     </row>
-    <row r="315" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A315" s="2" t="s">
         <v>93</v>
       </c>
       <c r="B315" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C315" s="2" t="s">
         <v>178</v>
@@ -6992,12 +6890,12 @@
         <v>198</v>
       </c>
     </row>
-    <row r="316" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A316" s="2" t="s">
         <v>93</v>
       </c>
       <c r="B316" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C316" s="2" t="s">
         <v>176</v>
@@ -7007,46 +6905,46 @@
         <v>176</v>
       </c>
     </row>
-    <row r="317" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A317" s="2" t="s">
         <v>94</v>
       </c>
       <c r="B317" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C317" s="2" t="s">
         <v>366</v>
       </c>
       <c r="D317" s="2" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="E317" s="2" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="318" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A318" s="2" t="s">
         <v>94</v>
       </c>
       <c r="B318" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C318" s="2" t="s">
         <v>367</v>
       </c>
       <c r="D318" s="2" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="E318" s="2" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="319" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A319" s="2" t="s">
         <v>94</v>
       </c>
       <c r="B319" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C319" s="2" t="s">
         <v>368</v>
@@ -7056,29 +6954,29 @@
         <v>197</v>
       </c>
     </row>
-    <row r="320" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A320" s="2" t="s">
         <v>94</v>
       </c>
       <c r="B320" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C320" s="2" t="s">
         <v>369</v>
       </c>
       <c r="D320" s="2" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="E320" s="2" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="321" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="321" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A321" s="2" t="s">
         <v>94</v>
       </c>
       <c r="B321" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C321" s="2" t="s">
         <v>191</v>
@@ -7092,9 +6990,7 @@
       <c r="A322" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B322" s="2" t="s">
-        <v>154</v>
-      </c>
+      <c r="B322" s="2"/>
       <c r="C322" s="2"/>
       <c r="D322" s="2"/>
       <c r="E322" s="2"/>
@@ -7109,7 +7005,7 @@
       </c>
       <c r="D323" s="2"/>
       <c r="E323" s="2" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
     </row>
     <row r="324" spans="1:5" x14ac:dyDescent="0.25">
@@ -7137,7 +7033,7 @@
       </c>
       <c r="D325" s="2"/>
       <c r="E325" s="2" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
     </row>
     <row r="326" spans="1:5" x14ac:dyDescent="0.25">
@@ -7149,10 +7045,10 @@
         <v>372</v>
       </c>
       <c r="D326" s="2" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="E326" s="2" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
     </row>
     <row r="327" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -7160,7 +7056,7 @@
         <v>98</v>
       </c>
       <c r="B327" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C327" s="2"/>
       <c r="D327" s="2"/>
@@ -7171,7 +7067,7 @@
         <v>99</v>
       </c>
       <c r="B328" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C328" s="2" t="s">
         <v>297</v>
@@ -7330,16 +7226,16 @@
         <v>100</v>
       </c>
       <c r="B339" s="2" t="s">
-        <v>539</v>
+        <v>172</v>
       </c>
       <c r="C339" s="2" t="s">
         <v>373</v>
       </c>
       <c r="D339" s="2" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="E339" s="2" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
     </row>
     <row r="340" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -7347,7 +7243,7 @@
         <v>100</v>
       </c>
       <c r="B340" s="2" t="s">
-        <v>539</v>
+        <v>172</v>
       </c>
       <c r="C340" s="2" t="s">
         <v>374</v>

</xml_diff>

<commit_message>
addition of adms and ifla
addition of adms and ifla
</commit_message>
<xml_diff>
--- a/v2.0.1/02-Glossary/ePO-Glossary.xlsx
+++ b/v2.0.1/02-Glossary/ePO-Glossary.xlsx
@@ -16187,4 +16187,210 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101001D0A01FC211A0A44AF46DCFC7788647F" ma:contentTypeVersion="6" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="cb8996f3c460f686c4ceead8a704479d">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8a9dc265-2a70-4a01-bf40-b0bb55b38d64" xmlns:ns3="56068758-a483-4a4b-84d7-1662caf98f10" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="319a6b9d4f2405982df31065c3fa6c19" ns2:_="" ns3:_="">
+    <xsd:import namespace="8a9dc265-2a70-4a01-bf40-b0bb55b38d64"/>
+    <xsd:import namespace="56068758-a483-4a4b-84d7-1662caf98f10"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="8a9dc265-2a70-4a01-bf40-b0bb55b38d64" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:description="" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:description="" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoTags" ma:description="" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="13" nillable="true" ma:displayName="MediaServiceOCR" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="56068758-a483-4a4b-84d7-1662caf98f10" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="11" nillable="true" ma:displayName="Compartido con" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="12" nillable="true" ma:displayName="Detalles de uso compartido" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo de contenido"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Título"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B7056DC-5189-4C60-ACF8-795E25874340}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D76B89A2-BE64-4875-BBE3-AA1D9821A596}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B25B31F0-17C1-4BED-A002-7337DA28B6C3}"/>
 </file>
</xml_diff>

<commit_message>
WG Meeting - review
</commit_message>
<xml_diff>
--- a/v2.0.1/02-Glossary/ePO-Glossary.xlsx
+++ b/v2.0.1/02-Glossary/ePO-Glossary.xlsx
@@ -17498,4 +17498,224 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001D0A01FC211A0A44AF46DCFC7788647F" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3bf4e89828d0d3cc2fc23292c739d613">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8a9dc265-2a70-4a01-bf40-b0bb55b38d64" xmlns:ns3="56068758-a483-4a4b-84d7-1662caf98f10" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ffc63a8b47298d93c51fdc2582bdfc36" ns2:_="" ns3:_="">
+    <xsd:import namespace="8a9dc265-2a70-4a01-bf40-b0bb55b38d64"/>
+    <xsd:import namespace="56068758-a483-4a4b-84d7-1662caf98f10"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="8a9dc265-2a70-4a01-bf40-b0bb55b38d64" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:description="" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:description="" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoTags" ma:description="" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="13" nillable="true" ma:displayName="MediaServiceOCR" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="14" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="15" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="56068758-a483-4a4b-84d7-1662caf98f10" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="11" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="12" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4EDA8ADC-AD37-4DD9-BC39-F65CDDDE3BBE}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{934275A9-B475-435D-A0F0-94EFD4C69FCF}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E92BE6C-AAE3-4AF9-A67D-30F767C19908}"/>
 </file>
</xml_diff>